<commit_message>
feat: add logo glitch effect, fix excel data mapping, and refine mobile typography
</commit_message>
<xml_diff>
--- a/public/items.xlsx
+++ b/public/items.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10005" windowHeight="16440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10000" windowHeight="20000" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Items" sheetId="1" r:id="rId1"/>
-    <sheet name="Values" sheetId="2" state="hidden" r:id="rId2"/>
-    <sheet name="Instructions" sheetId="3" r:id="rId3"/>
+    <sheet sheetId="1" name="Items" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Values" state="hidden" r:id="rId5"/>
+    <sheet sheetId="3" name="Instructions" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="68">
   <si>
     <t>CategoryID</t>
   </si>
@@ -36,15 +36,21 @@
     <t>ItemLink</t>
   </si>
   <si>
-    <t>ItemDescription</t>
-  </si>
-  <si>
     <t>CategoryTitle (Ref)</t>
   </si>
   <si>
     <t>TabLabel (Ref)</t>
   </si>
   <si>
+    <t>CategoryDesc</t>
+  </si>
+  <si>
+    <t>CategoryImg</t>
+  </si>
+  <si>
+    <t>CategoryBanner</t>
+  </si>
+  <si>
     <t>historic</t>
   </si>
   <si>
@@ -63,15 +69,15 @@
     <t>#</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Histórico</t>
   </si>
   <si>
     <t>Ruinas y Arquitectura</t>
   </si>
   <si>
+    <t>Explora mundos históricos con assets detallados de civilizaciones antiguas.</t>
+  </si>
+  <si>
     <t>artifacts</t>
   </si>
   <si>
@@ -108,6 +114,9 @@
     <t>Vehículos</t>
   </si>
   <si>
+    <t>Assets contemporáneos para ciudades y entornos urbanos modernos.</t>
+  </si>
+  <si>
     <t>tech</t>
   </si>
   <si>
@@ -142,6 +151,12 @@
   </si>
   <si>
     <t>Cyberpunk</t>
+  </si>
+  <si>
+    <t>Vehículos, mechas y tecnología del futuro para tus proyectos sci-fi.</t>
+  </si>
+  <si>
+    <t>media/scifi_card.png</t>
   </si>
   <si>
     <t>Dron de Asalto</t>
@@ -210,33 +225,30 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <color rgb="FFFFFFFF"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FFFFFFFF"/>
       <sz val="16"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <sz val="12"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,12 +263,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFAFAFA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -287,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -307,9 +313,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,18 +652,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="1"/>
   <cols>
-    <col min="1" max="9" width="25" customWidth="1"/>
+    <col min="1" max="11" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" ht="30" customHeight="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -682,278 +683,364 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="B3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="K3" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="6" t="s">
+      <c r="G4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="4" t="s">
+      <c r="G5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K5" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="C7" s="6" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="H7" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="I7" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="J8" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K8" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
+      <c r="J9" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Category" error="Select from list.">
-          <x14:formula1>
-            <xm:f>Values!$A$2:$A$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>A10:A158</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Category" error="Select from list.">
-          <x14:formula1>
-            <xm:f>Values!$A$2:$A$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>A2:A158</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Tab" error="Select from list.">
-          <x14:formula1>
-            <xm:f>Values!$B$2:$B$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>B10:B158</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Tab" error="Select from list.">
-          <x14:formula1>
-            <xm:f>Values!$B$2:$B$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B158</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="warning" errorTitle="Invalid Category" error="Select from list." sqref="A10:A59">
+      <formula1>'Values'!$A$2:$A$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="warning" errorTitle="Invalid Category" error="Select from list." sqref="A2:A59">
+      <formula1>'Values'!$A$2:$A$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="warning" errorTitle="Invalid Tab" error="Select from list." sqref="B10:B59">
+      <formula1>'Values'!$B$2:$B$7</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="warning" errorTitle="Invalid Tab" error="Select from list." sqref="B2:B59">
+      <formula1>'Values'!$B$2:$B$7</formula1>
+    </dataValidation>
+  </dataValidations>
 </worksheet>
 </file>
 
@@ -961,60 +1048,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
@@ -1022,50 +1108,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="1"/>
   <cols>
     <col min="1" max="1" width="80" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" ht="40" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>